<commit_message>
Aufbau und durchfuehrung gemacht
</commit_message>
<xml_diff>
--- a/Versuch424-Hall-Effekt-in-Halbleitern/Report/Tables/Day1-2.xlsx
+++ b/Versuch424-Hall-Effekt-in-Halbleitern/Report/Tables/Day1-2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>mess nr.</t>
   </si>
@@ -72,19 +72,31 @@
     <t>average</t>
   </si>
   <si>
-    <t>messung nr</t>
-  </si>
-  <si>
     <t>15,007 mA</t>
   </si>
   <si>
-    <t>temperatur1</t>
+    <t>B+</t>
   </si>
   <si>
-    <t>temperatur2</t>
+    <t>B-</t>
   </si>
   <si>
-    <t>Aver. Temp</t>
+    <t>t_1</t>
+  </si>
+  <si>
+    <t>t_2</t>
+  </si>
+  <si>
+    <t>&lt;t&gt;</t>
+  </si>
+  <si>
+    <t>Schaltung</t>
+  </si>
+  <si>
+    <t>$U / mV$</t>
+  </si>
+  <si>
+    <t>Messung</t>
   </si>
 </sst>
 </file>
@@ -429,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="I21" sqref="A12:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +456,7 @@
     <col min="5" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +470,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -486,7 +498,7 @@
         <v>4.0000000000000034E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -506,15 +518,15 @@
         <v>0.24099999999999999</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G21" si="0">AVERAGE(B3:F3)</f>
+        <f t="shared" ref="G3:H21" si="0">AVERAGE(B3:F3)</f>
         <v>0.24139999999999998</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H21" si="1">_xlfn.STDEV.P(B3:F3)</f>
+        <f t="shared" ref="H3:I21" si="1">_xlfn.STDEV.P(B3:F3)</f>
         <v>4.8989794855663611E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -542,7 +554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -570,7 +582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -598,7 +610,7 @@
         <v>4.0000000000000034E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -626,7 +638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -654,7 +666,7 @@
         <v>4.8989794855663611E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -682,17 +694,17 @@
         <v>4.89897948556636E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
-      <c r="B12">
-        <v>-8.0000000000000002E-3</v>
+      <c r="B12" t="s">
+        <v>19</v>
       </c>
       <c r="C12">
         <v>-8.0000000000000002E-3</v>
@@ -701,29 +713,32 @@
         <v>-8.0000000000000002E-3</v>
       </c>
       <c r="E12">
-        <v>-7.0000000000000001E-3</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
       <c r="F12">
         <v>-7.0000000000000001E-3</v>
       </c>
       <c r="G12">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="0"/>
         <v>-7.6E-3</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <f t="shared" si="1"/>
         <v>4.8989794855663557E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
         <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C13">
-        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D13">
         <v>6.0000000000000001E-3</v>
@@ -735,20 +750,23 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="G13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="0"/>
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <f t="shared" si="1"/>
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
-      <c r="B14">
-        <v>9.4E-2</v>
+      <c r="B14" t="s">
+        <v>19</v>
       </c>
       <c r="C14">
         <v>9.4E-2</v>
@@ -757,110 +775,122 @@
         <v>9.4E-2</v>
       </c>
       <c r="E14">
-        <v>9.5000000000000001E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="F14">
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="G14">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>9.4399999999999998E-2</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <f t="shared" si="1"/>
         <v>4.89897948556636E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15">
         <v>-9.7000000000000003E-2</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>-9.6000000000000002E-2</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>-9.6500000000000002E-2</v>
-      </c>
-      <c r="E15">
-        <v>-9.6000000000000002E-2</v>
       </c>
       <c r="F15">
         <v>-9.6000000000000002E-2</v>
       </c>
       <c r="G15">
+        <v>-9.6000000000000002E-2</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>-9.6299999999999983E-2</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <f t="shared" si="1"/>
         <v>4.0000000000000034E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
         <v>-9.6000000000000002E-2</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>-9.7000000000000003E-2</v>
-      </c>
-      <c r="D16">
-        <v>-9.6000000000000002E-2</v>
       </c>
       <c r="E16">
         <v>-9.6000000000000002E-2</v>
       </c>
       <c r="F16">
+        <v>-9.6000000000000002E-2</v>
+      </c>
+      <c r="G16">
         <v>-9.5000000000000001E-2</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <f t="shared" si="0"/>
         <v>-9.6000000000000002E-2</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <f t="shared" si="1"/>
         <v>6.3245553203367642E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17">
         <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="C17">
-        <v>9.5000000000000001E-2</v>
       </c>
       <c r="D17">
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="E17">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="F17">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <f t="shared" si="0"/>
         <v>8.7399999999999992E-2</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <f t="shared" si="1"/>
         <v>1.5704776343520507E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7</v>
       </c>
-      <c r="B18">
-        <v>5.0000000000000001E-3</v>
+      <c r="B18" t="s">
+        <v>20</v>
       </c>
       <c r="C18">
         <v>5.0000000000000001E-3</v>
@@ -872,23 +902,26 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G18">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <f t="shared" si="0"/>
         <v>5.2000000000000006E-3</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <f t="shared" si="1"/>
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>8</v>
       </c>
-      <c r="B19">
-        <v>-8.0000000000000002E-3</v>
+      <c r="B19" t="s">
+        <v>20</v>
       </c>
       <c r="C19">
         <v>-8.0000000000000002E-3</v>
@@ -900,23 +933,26 @@
         <v>-8.0000000000000002E-3</v>
       </c>
       <c r="F19">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="G19">
         <v>-7.0000000000000001E-3</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <f t="shared" si="0"/>
         <v>-7.7999999999999996E-3</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <f t="shared" si="1"/>
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9</v>
       </c>
       <c r="B20">
-        <v>-5.0999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="C20">
         <v>-5.0999999999999997E-2</v>
@@ -928,23 +964,26 @@
         <v>-5.0999999999999997E-2</v>
       </c>
       <c r="F20">
+        <v>-5.0999999999999997E-2</v>
+      </c>
+      <c r="G20">
         <v>-0.05</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <f t="shared" si="0"/>
         <v>-5.0799999999999998E-2</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <f t="shared" si="1"/>
         <v>3.9999999999999758E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10</v>
       </c>
       <c r="B21">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C21">
         <v>0.05</v>
@@ -956,13 +995,16 @@
         <v>0.05</v>
       </c>
       <c r="F21">
+        <v>0.05</v>
+      </c>
+      <c r="G21">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <f t="shared" si="0"/>
         <v>5.0200000000000002E-2</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <f t="shared" si="1"/>
         <v>3.9999999999999758E-4</v>
       </c>
@@ -970,17 +1012,17 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="G3:H21 G2:H2" formulaRange="1"/>
+    <ignoredError sqref="H12:I21 G2:H11" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I23" sqref="A14:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,7 +1034,7 @@
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1012,7 +1054,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1035,7 +1077,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1063,7 +1105,7 @@
         <v>8.1092539730842923E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1083,15 +1125,15 @@
         <v>89.867999999999995</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G23" si="0">AVERAGE(B5:F5)</f>
+        <f t="shared" ref="G5:H23" si="0">AVERAGE(B5:F5)</f>
         <v>89.862399999999994</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H23" si="1">_xlfn.STDEV.P(B5:F5)</f>
+        <f t="shared" ref="H5:I23" si="1">_xlfn.STDEV.P(B5:F5)</f>
         <v>7.3102667529985847E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1119,7 +1161,7 @@
         <v>6.2801273872456842E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1147,7 +1189,7 @@
         <v>6.2417946137332857E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1175,7 +1217,7 @@
         <v>5.7758116312787615E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1203,7 +1245,7 @@
         <v>5.2000000000013268E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1231,7 +1273,7 @@
         <v>4.4452221541761419E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1259,7 +1301,7 @@
         <v>4.7074409183775149E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1279,282 +1321,312 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1">
         <v>26.524000000000001</v>
-      </c>
-      <c r="C14" s="1">
-        <v>26.515999999999998</v>
       </c>
       <c r="D14" s="1">
         <v>26.515999999999998</v>
       </c>
       <c r="E14" s="1">
+        <v>26.515999999999998</v>
+      </c>
+      <c r="F14" s="1">
         <v>26.513000000000002</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>26.498999999999999</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>26.513600000000004</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <f t="shared" si="1"/>
         <v>8.1633326527838588E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1">
         <v>-26.462</v>
-      </c>
-      <c r="C15" s="1">
-        <v>-26.454000000000001</v>
       </c>
       <c r="D15" s="1">
         <v>-26.454000000000001</v>
       </c>
       <c r="E15" s="1">
+        <v>-26.454000000000001</v>
+      </c>
+      <c r="F15" s="1">
         <v>-26.451000000000001</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>-26.437000000000001</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>-26.451600000000003</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <f t="shared" si="1"/>
         <v>8.1633326527830053E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>3</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1">
         <v>27.192</v>
-      </c>
-      <c r="C16" s="1">
-        <v>27.184000000000001</v>
       </c>
       <c r="D16" s="1">
         <v>27.184000000000001</v>
       </c>
       <c r="E16" s="1">
+        <v>27.184000000000001</v>
+      </c>
+      <c r="F16" s="1">
         <v>27.181999999999999</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>27.169</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <f t="shared" si="0"/>
         <v>27.182200000000002</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <f t="shared" si="1"/>
         <v>7.4404300950952924E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>4</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="1">
         <v>-27.202999999999999</v>
-      </c>
-      <c r="C17" s="1">
-        <v>-27.193999999999999</v>
       </c>
       <c r="D17" s="1">
         <v>-27.193999999999999</v>
       </c>
       <c r="E17" s="1">
+        <v>-27.193999999999999</v>
+      </c>
+      <c r="F17" s="1">
         <v>-27.192</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>-27.178000000000001</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <f t="shared" si="0"/>
         <v>-27.192199999999996</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <f t="shared" si="1"/>
         <v>8.0597766718434188E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>5</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="1">
         <v>-27.196000000000002</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>-27.199000000000002</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>-27.193000000000001</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>-27.187000000000001</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>-27.18</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <f t="shared" si="0"/>
         <v>-27.191000000000003</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <f t="shared" si="1"/>
         <v>6.7823299831259089E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>6</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1">
         <v>27.26</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D19" s="1">
         <v>27.263000000000002</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>27.257000000000001</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>27.25</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>27.242999999999999</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <f t="shared" si="0"/>
         <v>27.2546</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <f t="shared" si="1"/>
         <v>7.2277243998382455E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>7</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1">
         <v>-26.501000000000001</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>-26.504000000000001</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>-26.495999999999999</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>-26.49</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>-26.484000000000002</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <f t="shared" si="0"/>
         <v>-26.494999999999997</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <f t="shared" si="1"/>
         <v>7.2663608498341583E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>8</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1">
         <v>26.495000000000001</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21" s="1">
         <v>26.498999999999999</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>26.492000000000001</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <v>26.486000000000001</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1">
         <v>26.478999999999999</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <f t="shared" si="0"/>
         <v>26.490200000000005</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <f t="shared" si="1"/>
         <v>7.0256672281001683E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>9</v>
       </c>
-      <c r="B22" s="1">
-        <v>-0.33</v>
+      <c r="B22">
+        <v>0</v>
       </c>
       <c r="C22" s="1">
         <v>-0.33</v>
       </c>
       <c r="D22" s="1">
+        <v>-0.33</v>
+      </c>
+      <c r="E22" s="1">
         <v>-0.33100000000000002</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <v>-0.32900000000000001</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>-0.33100000000000002</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <f t="shared" si="0"/>
         <v>-0.33019999999999999</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <f t="shared" si="1"/>
         <v>7.4833147735478892E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>10</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
         <v>0.39400000000000002</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0.39300000000000002</v>
       </c>
       <c r="D23" s="1">
         <v>0.39300000000000002</v>
       </c>
       <c r="E23" s="1">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="F23" s="1">
         <v>0.39400000000000002</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>0.39300000000000002</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <f t="shared" si="0"/>
         <v>0.39340000000000008</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <f t="shared" si="1"/>
         <v>4.89897948556636E-4</v>
       </c>
@@ -1562,81 +1634,94 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="G4:H23" formulaRange="1"/>
+    <ignoredError sqref="H14:I23 G4:H13" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F14:F15"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="15" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="15" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B1">
-        <v>-206</v>
+        <v>1</v>
       </c>
       <c r="C1">
-        <v>-196</v>
+        <v>2</v>
       </c>
       <c r="D1">
-        <v>-183</v>
+        <v>3</v>
       </c>
       <c r="E1">
-        <v>-172</v>
+        <v>4</v>
       </c>
       <c r="F1">
-        <v>-163</v>
+        <v>5</v>
       </c>
       <c r="G1">
-        <v>-153</v>
+        <v>6</v>
       </c>
       <c r="H1">
-        <v>-140</v>
+        <v>7</v>
       </c>
       <c r="I1">
-        <v>-125</v>
+        <v>8</v>
       </c>
       <c r="J1">
-        <v>-110</v>
+        <v>9</v>
       </c>
       <c r="K1">
-        <v>-93</v>
+        <v>10</v>
       </c>
       <c r="L1">
-        <v>-79</v>
+        <v>11</v>
       </c>
       <c r="M1">
-        <v>-64</v>
+        <v>12</v>
       </c>
       <c r="N1">
-        <v>-27</v>
+        <v>13</v>
       </c>
       <c r="O1">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
+      <c r="B2">
+        <v>-206</v>
+      </c>
+      <c r="C2">
+        <v>-196</v>
+      </c>
+      <c r="D2">
+        <v>-183</v>
+      </c>
+      <c r="E2">
+        <v>-172</v>
+      </c>
       <c r="F2">
-        <v>-160</v>
+        <v>-163</v>
       </c>
       <c r="G2">
-        <v>-151</v>
+        <v>-153</v>
       </c>
       <c r="H2">
         <v>-140</v>
@@ -1645,7 +1730,7 @@
         <v>-125</v>
       </c>
       <c r="J2">
-        <v>-109</v>
+        <v>-110</v>
       </c>
       <c r="K2">
         <v>-93</v>
@@ -1654,7 +1739,13 @@
         <v>-79</v>
       </c>
       <c r="M2">
-        <v>-62</v>
+        <v>-64</v>
+      </c>
+      <c r="N2">
+        <v>-27</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1662,958 +1753,1005 @@
         <v>22</v>
       </c>
       <c r="B3">
-        <f>AVERAGE(B1:B2)</f>
-        <v>-206</v>
+        <v>-205</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:O3" si="0">AVERAGE(C1:C2)</f>
-        <v>-196</v>
+        <v>-195</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
         <v>-183</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
-        <v>-172</v>
+        <v>-173</v>
       </c>
       <c r="F3">
-        <f t="shared" si="0"/>
-        <v>-161.5</v>
+        <v>-160</v>
       </c>
       <c r="G3">
-        <f t="shared" si="0"/>
-        <v>-152</v>
+        <v>-151</v>
       </c>
       <c r="H3">
-        <f t="shared" si="0"/>
         <v>-140</v>
       </c>
       <c r="I3">
-        <f t="shared" si="0"/>
         <v>-125</v>
       </c>
       <c r="J3">
-        <f t="shared" si="0"/>
-        <v>-109.5</v>
+        <v>-109</v>
       </c>
       <c r="K3">
-        <f t="shared" si="0"/>
         <v>-93</v>
       </c>
       <c r="L3">
-        <f t="shared" si="0"/>
         <v>-79</v>
       </c>
       <c r="M3">
-        <f t="shared" si="0"/>
-        <v>-63</v>
+        <v>-62</v>
       </c>
       <c r="N3">
-        <f t="shared" si="0"/>
         <v>-27</v>
       </c>
       <c r="O3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <f>AVERAGE(B2:B3)</f>
+        <v>-205.5</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:O4" si="0">AVERAGE(C2:C3)</f>
+        <v>-195.5</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>-183</v>
+      </c>
+      <c r="E4">
+        <f>AVERAGE(E2:E3)</f>
+        <v>-172.5</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>-161.5</v>
       </c>
       <c r="G4">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>-152</v>
       </c>
       <c r="H4">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>-140</v>
       </c>
       <c r="I4">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>-125</v>
       </c>
       <c r="J4">
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>-109.5</v>
       </c>
       <c r="K4">
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>-93</v>
       </c>
       <c r="L4">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>-79</v>
       </c>
       <c r="M4">
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>-63</v>
       </c>
       <c r="N4">
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>-27</v>
       </c>
       <c r="O4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>-82.382000000000005</v>
-      </c>
-      <c r="C5">
-        <v>-82.54</v>
-      </c>
-      <c r="D5">
-        <v>-82.9</v>
-      </c>
-      <c r="E5">
-        <v>-83.3</v>
-      </c>
-      <c r="F5">
-        <v>-83.596000000000004</v>
-      </c>
-      <c r="G5">
-        <v>-83.793000000000006</v>
-      </c>
-      <c r="H5">
-        <v>-84.02</v>
-      </c>
-      <c r="I5">
-        <v>-84.54</v>
-      </c>
-      <c r="J5">
-        <v>-85.194999999999993</v>
-      </c>
-      <c r="K5">
-        <v>-85.71</v>
-      </c>
-      <c r="L5">
-        <v>-86.432000000000002</v>
-      </c>
-      <c r="M5">
-        <v>-87.257999999999996</v>
-      </c>
-      <c r="N5">
-        <v>-88.869</v>
-      </c>
-      <c r="O5">
-        <v>-90.2</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>82.504999999999995</v>
-      </c>
-      <c r="C6">
-        <v>82.665000000000006</v>
-      </c>
-      <c r="D6">
-        <v>83.027000000000001</v>
-      </c>
-      <c r="E6">
-        <v>83.412000000000006</v>
-      </c>
-      <c r="F6">
-        <v>83.712000000000003</v>
-      </c>
-      <c r="G6">
-        <v>83.9</v>
-      </c>
-      <c r="H6">
-        <v>84.12</v>
-      </c>
-      <c r="I6">
-        <v>84.614999999999995</v>
-      </c>
-      <c r="J6">
-        <v>85.274000000000001</v>
-      </c>
-      <c r="K6">
-        <v>85.75</v>
-      </c>
-      <c r="L6">
-        <v>86.475999999999999</v>
-      </c>
-      <c r="M6">
-        <v>87.287999999999997</v>
-      </c>
-      <c r="N6">
-        <v>88.869</v>
-      </c>
-      <c r="O6">
-        <v>90.165999999999997</v>
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>-82.076999999999998</v>
+        <v>-82.382000000000005</v>
       </c>
       <c r="C7">
-        <v>-82.24</v>
+        <v>-82.54</v>
       </c>
       <c r="D7">
-        <v>-82.608000000000004</v>
+        <v>-82.9</v>
       </c>
       <c r="E7">
-        <v>-82.986999999999995</v>
+        <v>-83.3</v>
       </c>
       <c r="F7">
-        <v>-83.305000000000007</v>
+        <v>-83.596000000000004</v>
       </c>
       <c r="G7">
-        <v>-83.495000000000005</v>
+        <v>-83.793000000000006</v>
       </c>
       <c r="H7">
-        <v>-83.713999999999999</v>
+        <v>-84.02</v>
       </c>
       <c r="I7">
-        <v>-84.2</v>
+        <v>-84.54</v>
       </c>
       <c r="J7">
-        <v>-84.888000000000005</v>
+        <v>-85.194999999999993</v>
       </c>
       <c r="K7">
-        <v>-85.343999999999994</v>
+        <v>-85.71</v>
       </c>
       <c r="L7">
-        <v>-86.102000000000004</v>
+        <v>-86.432000000000002</v>
       </c>
       <c r="M7">
-        <v>-86.906999999999996</v>
+        <v>-87.257999999999996</v>
       </c>
       <c r="N7">
-        <v>-88.522999999999996</v>
+        <v>-88.869</v>
       </c>
       <c r="O7">
-        <v>-89.837000000000003</v>
+        <v>-90.2</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>82.111000000000004</v>
+        <v>82.504999999999995</v>
       </c>
       <c r="C8">
-        <v>82.277000000000001</v>
+        <v>82.665000000000006</v>
       </c>
       <c r="D8">
-        <v>82.65</v>
+        <v>83.027000000000001</v>
       </c>
       <c r="E8">
-        <v>83.025000000000006</v>
+        <v>83.412000000000006</v>
       </c>
       <c r="F8">
-        <v>83.320999999999998</v>
+        <v>83.712000000000003</v>
       </c>
       <c r="G8">
-        <v>83.55</v>
+        <v>83.9</v>
       </c>
       <c r="H8">
-        <v>83.754999999999995</v>
+        <v>84.12</v>
       </c>
       <c r="I8">
-        <v>84.227999999999994</v>
+        <v>84.614999999999995</v>
       </c>
       <c r="J8">
-        <v>84.927999999999997</v>
+        <v>85.274000000000001</v>
       </c>
       <c r="K8">
-        <v>85.372</v>
+        <v>85.75</v>
       </c>
       <c r="L8">
-        <v>86.129000000000005</v>
+        <v>86.475999999999999</v>
       </c>
       <c r="M8">
-        <v>86.924000000000007</v>
+        <v>87.287999999999997</v>
       </c>
       <c r="N8">
-        <v>88.527000000000001</v>
+        <v>88.869</v>
       </c>
       <c r="O8">
-        <v>89.802000000000007</v>
+        <v>90.165999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>-82.429000000000002</v>
+        <v>-82.076999999999998</v>
       </c>
       <c r="C9">
-        <v>-82.597999999999999</v>
+        <v>-82.24</v>
       </c>
       <c r="D9">
-        <v>-82.97</v>
+        <v>-82.608000000000004</v>
       </c>
       <c r="E9">
-        <v>-83.334999999999994</v>
+        <v>-82.986999999999995</v>
       </c>
       <c r="F9">
-        <v>-83.626999999999995</v>
+        <v>-83.305000000000007</v>
       </c>
       <c r="G9">
-        <v>-83.884</v>
+        <v>-83.495000000000005</v>
       </c>
       <c r="H9">
-        <v>-84.058000000000007</v>
+        <v>-83.713999999999999</v>
       </c>
       <c r="I9">
-        <v>-84.52</v>
+        <v>-84.2</v>
       </c>
       <c r="J9">
-        <v>-85.242999999999995</v>
+        <v>-84.888000000000005</v>
       </c>
       <c r="K9">
-        <v>-85.688000000000002</v>
+        <v>-85.343999999999994</v>
       </c>
       <c r="L9">
-        <v>-86.454999999999998</v>
+        <v>-86.102000000000004</v>
       </c>
       <c r="M9">
-        <v>-87.253</v>
+        <v>-86.906999999999996</v>
       </c>
       <c r="N9">
-        <v>-88.875</v>
+        <v>-88.522999999999996</v>
       </c>
       <c r="O9">
-        <v>-90.156999999999996</v>
+        <v>-89.837000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>82.457999999999998</v>
+        <v>82.111000000000004</v>
       </c>
       <c r="C10">
-        <v>82.622</v>
+        <v>82.277000000000001</v>
       </c>
       <c r="D10">
-        <v>82.99</v>
+        <v>82.65</v>
       </c>
       <c r="E10">
-        <v>83.349000000000004</v>
+        <v>83.025000000000006</v>
       </c>
       <c r="F10">
-        <v>83.64</v>
+        <v>83.320999999999998</v>
       </c>
       <c r="G10">
-        <v>83.902000000000001</v>
+        <v>83.55</v>
       </c>
       <c r="H10">
-        <v>84.066000000000003</v>
+        <v>83.754999999999995</v>
       </c>
       <c r="I10">
-        <v>84.513000000000005</v>
+        <v>84.227999999999994</v>
       </c>
       <c r="J10">
-        <v>85.251000000000005</v>
+        <v>84.927999999999997</v>
       </c>
       <c r="K10">
-        <v>85.692999999999998</v>
+        <v>85.372</v>
       </c>
       <c r="L10">
-        <v>86.462999999999994</v>
+        <v>86.129000000000005</v>
       </c>
       <c r="M10">
-        <v>87.265000000000001</v>
+        <v>86.924000000000007</v>
       </c>
       <c r="N10">
-        <v>88.91</v>
+        <v>88.527000000000001</v>
       </c>
       <c r="O10">
-        <v>90.182000000000002</v>
+        <v>89.802000000000007</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <v>-82.192999999999998</v>
+        <v>-82.429000000000002</v>
       </c>
       <c r="C11">
-        <v>-82.364000000000004</v>
+        <v>-82.597999999999999</v>
       </c>
       <c r="D11">
-        <v>-82.73</v>
+        <v>-82.97</v>
       </c>
       <c r="E11">
-        <v>-83.081000000000003</v>
+        <v>-83.334999999999994</v>
       </c>
       <c r="F11">
-        <v>-83.378</v>
+        <v>-83.626999999999995</v>
       </c>
       <c r="G11">
-        <v>-83.63</v>
+        <v>-83.884</v>
       </c>
       <c r="H11">
-        <v>-83.786000000000001</v>
+        <v>-84.058000000000007</v>
       </c>
       <c r="I11">
-        <v>-84.222999999999999</v>
+        <v>-84.52</v>
       </c>
       <c r="J11">
-        <v>-84.933999999999997</v>
+        <v>-85.242999999999995</v>
       </c>
       <c r="K11">
-        <v>-85.393000000000001</v>
+        <v>-85.688000000000002</v>
       </c>
       <c r="L11">
-        <v>-86.150999999999996</v>
+        <v>-86.454999999999998</v>
       </c>
       <c r="M11">
-        <v>-86.94</v>
+        <v>-87.253</v>
       </c>
       <c r="N11">
-        <v>-88.563000000000002</v>
+        <v>-88.875</v>
       </c>
       <c r="O11">
-        <v>-89.8</v>
+        <v>-90.156999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12">
-        <v>81.992000000000004</v>
+        <v>82.457999999999998</v>
       </c>
       <c r="C12">
-        <v>82.171999999999997</v>
+        <v>82.622</v>
       </c>
       <c r="D12">
-        <v>82.48</v>
+        <v>82.99</v>
       </c>
       <c r="E12">
-        <v>82.905000000000001</v>
+        <v>83.349000000000004</v>
       </c>
       <c r="F12">
-        <v>83.218000000000004</v>
+        <v>83.64</v>
       </c>
       <c r="G12">
-        <v>83.466999999999999</v>
+        <v>83.902000000000001</v>
       </c>
       <c r="H12">
-        <v>83.628</v>
+        <v>84.066000000000003</v>
       </c>
       <c r="I12">
-        <v>84.075999999999993</v>
+        <v>84.513000000000005</v>
       </c>
       <c r="J12">
-        <v>84.805000000000007</v>
+        <v>85.251000000000005</v>
       </c>
       <c r="K12">
-        <v>85.28</v>
+        <v>85.692999999999998</v>
       </c>
       <c r="L12">
-        <v>86.057000000000002</v>
+        <v>86.462999999999994</v>
       </c>
       <c r="M12">
-        <v>86.864999999999995</v>
+        <v>87.265000000000001</v>
       </c>
       <c r="N12">
-        <v>88.546999999999997</v>
+        <v>88.91</v>
       </c>
       <c r="O12">
-        <v>89.822999999999993</v>
+        <v>90.182000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>-82.192999999999998</v>
+      </c>
+      <c r="C13">
+        <v>-82.364000000000004</v>
+      </c>
+      <c r="D13">
+        <v>-82.73</v>
+      </c>
+      <c r="E13">
+        <v>-83.081000000000003</v>
+      </c>
+      <c r="F13">
+        <v>-83.378</v>
+      </c>
+      <c r="G13">
+        <v>-83.63</v>
+      </c>
+      <c r="H13">
+        <v>-83.786000000000001</v>
+      </c>
+      <c r="I13">
+        <v>-84.222999999999999</v>
+      </c>
+      <c r="J13">
+        <v>-84.933999999999997</v>
+      </c>
+      <c r="K13">
+        <v>-85.393000000000001</v>
+      </c>
+      <c r="L13">
+        <v>-86.150999999999996</v>
+      </c>
+      <c r="M13">
+        <v>-86.94</v>
+      </c>
+      <c r="N13">
+        <v>-88.563000000000002</v>
+      </c>
+      <c r="O13">
+        <v>-89.8</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B14">
-        <v>26.978000000000002</v>
+        <v>81.992000000000004</v>
       </c>
       <c r="C14">
-        <v>27.03</v>
+        <v>82.171999999999997</v>
       </c>
       <c r="D14">
-        <v>27.041</v>
+        <v>82.48</v>
       </c>
       <c r="E14">
-        <v>27.047999999999998</v>
+        <v>82.905000000000001</v>
       </c>
       <c r="F14">
-        <v>27.044</v>
+        <v>83.218000000000004</v>
       </c>
       <c r="G14">
-        <v>27.047000000000001</v>
+        <v>83.466999999999999</v>
       </c>
       <c r="H14">
-        <v>27.027999999999999</v>
+        <v>83.628</v>
       </c>
       <c r="I14">
-        <v>26.99</v>
+        <v>84.075999999999993</v>
       </c>
       <c r="J14">
-        <v>26.922000000000001</v>
+        <v>84.805000000000007</v>
       </c>
       <c r="K14">
-        <v>26.879000000000001</v>
+        <v>85.28</v>
       </c>
       <c r="L14">
-        <v>26.831</v>
+        <v>86.057000000000002</v>
       </c>
       <c r="M14">
-        <v>26.779</v>
+        <v>86.864999999999995</v>
       </c>
       <c r="N14">
-        <v>26.620999999999999</v>
+        <v>88.546999999999997</v>
       </c>
       <c r="O14">
-        <v>26.483000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15">
-        <v>-27.15</v>
-      </c>
-      <c r="C15">
-        <v>-27.204999999999998</v>
-      </c>
-      <c r="D15">
-        <v>-27.213999999999999</v>
-      </c>
-      <c r="E15">
-        <v>-27.219000000000001</v>
-      </c>
-      <c r="F15">
-        <v>-27.2</v>
-      </c>
-      <c r="G15">
-        <v>-27.196999999999999</v>
-      </c>
-      <c r="H15">
-        <v>-27.172999999999998</v>
-      </c>
-      <c r="I15">
-        <v>-27.126999999999999</v>
-      </c>
-      <c r="J15">
-        <v>-27.04</v>
-      </c>
-      <c r="K15">
-        <v>-26.983000000000001</v>
-      </c>
-      <c r="L15">
-        <v>-26.916</v>
-      </c>
-      <c r="M15">
-        <v>-26.85</v>
-      </c>
-      <c r="N15">
-        <v>-26.63</v>
-      </c>
-      <c r="O15">
-        <v>-26.443000000000001</v>
+        <v>89.822999999999993</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B16">
-        <v>27.808</v>
+        <v>26.978000000000002</v>
       </c>
       <c r="C16">
-        <v>27.849</v>
+        <v>27.03</v>
       </c>
       <c r="D16">
-        <v>27.847999999999999</v>
+        <v>27.041</v>
       </c>
       <c r="E16">
-        <v>27.85</v>
+        <v>27.047999999999998</v>
       </c>
       <c r="F16">
-        <v>27.832000000000001</v>
+        <v>27.044</v>
       </c>
       <c r="G16">
-        <v>27.827999999999999</v>
+        <v>27.047000000000001</v>
       </c>
       <c r="H16">
-        <v>27.806000000000001</v>
+        <v>27.027999999999999</v>
       </c>
       <c r="I16">
-        <v>27.760999999999999</v>
+        <v>26.99</v>
       </c>
       <c r="J16">
-        <v>27.684000000000001</v>
+        <v>26.922000000000001</v>
       </c>
       <c r="K16">
-        <v>27.631</v>
+        <v>26.879000000000001</v>
       </c>
       <c r="L16">
-        <v>27.573</v>
+        <v>26.831</v>
       </c>
       <c r="M16">
-        <v>27.518000000000001</v>
+        <v>26.779</v>
       </c>
       <c r="N16">
-        <v>27.317</v>
+        <v>26.620999999999999</v>
       </c>
       <c r="O16">
-        <v>27.154</v>
+        <v>26.483000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B17">
-        <v>-27.742000000000001</v>
+        <v>-27.15</v>
       </c>
       <c r="C17">
-        <v>-27.786999999999999</v>
+        <v>-27.204999999999998</v>
       </c>
       <c r="D17">
-        <v>-27.786000000000001</v>
+        <v>-27.213999999999999</v>
       </c>
       <c r="E17">
-        <v>-27.789000000000001</v>
+        <v>-27.219000000000001</v>
       </c>
       <c r="F17">
-        <v>-27.774999999999999</v>
+        <v>-27.2</v>
       </c>
       <c r="G17">
-        <v>-27.771000000000001</v>
+        <v>-27.196999999999999</v>
       </c>
       <c r="H17">
-        <v>-27.745999999999999</v>
+        <v>-27.172999999999998</v>
       </c>
       <c r="I17">
-        <v>-27.707000000000001</v>
+        <v>-27.126999999999999</v>
       </c>
       <c r="J17">
-        <v>-27.63</v>
+        <v>-27.04</v>
       </c>
       <c r="K17">
-        <v>-27.584</v>
+        <v>-26.983000000000001</v>
       </c>
       <c r="L17">
-        <v>-27.533000000000001</v>
+        <v>-26.916</v>
       </c>
       <c r="M17">
-        <v>-27.481000000000002</v>
+        <v>-26.85</v>
       </c>
       <c r="N17">
-        <v>-27.303000000000001</v>
+        <v>-26.63</v>
       </c>
       <c r="O17">
-        <v>-27.16</v>
+        <v>-26.443000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B18">
-        <v>-27.888999999999999</v>
+        <v>27.808</v>
       </c>
       <c r="C18">
-        <v>-27.922999999999998</v>
+        <v>27.849</v>
       </c>
       <c r="D18">
-        <v>-27.940999999999999</v>
+        <v>27.847999999999999</v>
       </c>
       <c r="E18">
-        <v>-27.937999999999999</v>
+        <v>27.85</v>
       </c>
       <c r="F18">
-        <v>-27.914000000000001</v>
+        <v>27.832000000000001</v>
       </c>
       <c r="G18">
-        <v>-27.914000000000001</v>
+        <v>27.827999999999999</v>
       </c>
       <c r="H18">
-        <v>-27.88</v>
+        <v>27.806000000000001</v>
       </c>
       <c r="I18">
-        <v>-27.832000000000001</v>
+        <v>27.760999999999999</v>
       </c>
       <c r="J18">
-        <v>-27.754000000000001</v>
+        <v>27.684000000000001</v>
       </c>
       <c r="K18">
-        <v>-27.7</v>
+        <v>27.631</v>
       </c>
       <c r="L18">
-        <v>-27.638999999999999</v>
+        <v>27.573</v>
       </c>
       <c r="M18">
-        <v>-27.562999999999999</v>
+        <v>27.518000000000001</v>
       </c>
       <c r="N18">
-        <v>-27.352</v>
+        <v>27.317</v>
       </c>
       <c r="O18">
-        <v>-27.177</v>
+        <v>27.154</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B19">
-        <v>27.722000000000001</v>
+        <v>-27.742000000000001</v>
       </c>
       <c r="C19">
-        <v>27.751999999999999</v>
+        <v>-27.786999999999999</v>
       </c>
       <c r="D19">
-        <v>27.773</v>
+        <v>-27.786000000000001</v>
       </c>
       <c r="E19">
-        <v>27.774000000000001</v>
+        <v>-27.789000000000001</v>
       </c>
       <c r="F19">
-        <v>27.760999999999999</v>
+        <v>-27.774999999999999</v>
       </c>
       <c r="G19">
-        <v>27.765999999999998</v>
+        <v>-27.771000000000001</v>
       </c>
       <c r="H19">
-        <v>27.74</v>
+        <v>-27.745999999999999</v>
       </c>
       <c r="I19">
-        <v>27.699000000000002</v>
+        <v>-27.707000000000001</v>
       </c>
       <c r="J19">
-        <v>27.641999999999999</v>
+        <v>-27.63</v>
       </c>
       <c r="K19">
-        <v>27.6</v>
+        <v>-27.584</v>
       </c>
       <c r="L19">
-        <v>27.558</v>
+        <v>-27.533000000000001</v>
       </c>
       <c r="M19">
-        <v>27.5</v>
+        <v>-27.481000000000002</v>
       </c>
       <c r="N19">
-        <v>27.344999999999999</v>
+        <v>-27.303000000000001</v>
       </c>
       <c r="O19">
-        <v>27.219000000000001</v>
+        <v>-27.16</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B20">
-        <v>-27.085000000000001</v>
+        <v>-27.888999999999999</v>
       </c>
       <c r="C20">
-        <v>-27.12</v>
+        <v>-27.922999999999998</v>
       </c>
       <c r="D20">
-        <v>-27.14</v>
+        <v>-27.940999999999999</v>
       </c>
       <c r="E20">
-        <v>-27.143000000000001</v>
+        <v>-27.937999999999999</v>
       </c>
       <c r="F20">
-        <v>-27.122</v>
+        <v>-27.914000000000001</v>
       </c>
       <c r="G20">
-        <v>-27.125</v>
+        <v>-27.914000000000001</v>
       </c>
       <c r="H20">
-        <v>-27.094999999999999</v>
+        <v>-27.88</v>
       </c>
       <c r="I20">
-        <v>-27.052</v>
+        <v>-27.832000000000001</v>
       </c>
       <c r="J20">
-        <v>-26.98</v>
+        <v>-27.754000000000001</v>
       </c>
       <c r="K20">
-        <v>-26.928000000000001</v>
+        <v>-27.7</v>
       </c>
       <c r="L20">
-        <v>-26.88</v>
+        <v>-27.638999999999999</v>
       </c>
       <c r="M20">
-        <v>-26.811</v>
+        <v>-27.562999999999999</v>
       </c>
       <c r="N20">
-        <v>-26.628</v>
+        <v>-27.352</v>
       </c>
       <c r="O20">
-        <v>-26.48</v>
+        <v>-27.177</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B21">
-        <v>27.15</v>
+        <v>27.722000000000001</v>
       </c>
       <c r="C21">
-        <v>27.18</v>
+        <v>27.751999999999999</v>
       </c>
       <c r="D21">
-        <v>27.198</v>
+        <v>27.773</v>
       </c>
       <c r="E21">
-        <v>27.199000000000002</v>
+        <v>27.774000000000001</v>
       </c>
       <c r="F21">
-        <v>27.175000000000001</v>
+        <v>27.760999999999999</v>
       </c>
       <c r="G21">
-        <v>27.177</v>
+        <v>27.765999999999998</v>
       </c>
       <c r="H21">
-        <v>27.15</v>
+        <v>27.74</v>
       </c>
       <c r="I21">
-        <v>27.100999999999999</v>
+        <v>27.699000000000002</v>
       </c>
       <c r="J21">
-        <v>27.027999999999999</v>
+        <v>27.641999999999999</v>
       </c>
       <c r="K21">
-        <v>26.972999999999999</v>
+        <v>27.6</v>
       </c>
       <c r="L21">
-        <v>26.917999999999999</v>
+        <v>27.558</v>
       </c>
       <c r="M21">
-        <v>26.841999999999999</v>
+        <v>27.5</v>
       </c>
       <c r="N21">
-        <v>26.641999999999999</v>
+        <v>27.344999999999999</v>
       </c>
       <c r="O21">
-        <v>26.471</v>
+        <v>27.219000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B22">
-        <v>-0.44</v>
+        <v>-27.085000000000001</v>
       </c>
       <c r="C22">
-        <v>-0.439</v>
+        <v>-27.12</v>
       </c>
       <c r="D22">
-        <v>-0.435</v>
+        <v>-27.14</v>
       </c>
       <c r="E22">
-        <v>-0.43099999999999999</v>
+        <v>-27.143000000000001</v>
       </c>
       <c r="F22">
-        <v>-0.42599999999999999</v>
+        <v>-27.122</v>
       </c>
       <c r="G22">
-        <v>-0.42099999999999999</v>
+        <v>-27.125</v>
       </c>
       <c r="H22">
-        <v>-0.41599999999999998</v>
+        <v>-27.094999999999999</v>
       </c>
       <c r="I22">
-        <v>-0.41399999999999998</v>
+        <v>-27.052</v>
       </c>
       <c r="J22">
-        <v>-0.40400000000000003</v>
+        <v>-26.98</v>
       </c>
       <c r="K22">
-        <v>-0.39900000000000002</v>
+        <v>-26.928000000000001</v>
       </c>
       <c r="L22">
-        <v>-0.39100000000000001</v>
+        <v>-26.88</v>
       </c>
       <c r="M22">
-        <v>-0.38400000000000001</v>
+        <v>-26.811</v>
       </c>
       <c r="N22">
-        <v>-0.36</v>
+        <v>-26.628</v>
       </c>
       <c r="O22">
-        <v>-0.33900000000000002</v>
+        <v>-26.48</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>27.15</v>
+      </c>
+      <c r="C23">
+        <v>27.18</v>
+      </c>
+      <c r="D23">
+        <v>27.198</v>
+      </c>
+      <c r="E23">
+        <v>27.199000000000002</v>
+      </c>
+      <c r="F23">
+        <v>27.175000000000001</v>
+      </c>
+      <c r="G23">
+        <v>27.177</v>
+      </c>
+      <c r="H23">
+        <v>27.15</v>
+      </c>
+      <c r="I23">
+        <v>27.100999999999999</v>
+      </c>
+      <c r="J23">
+        <v>27.027999999999999</v>
+      </c>
+      <c r="K23">
+        <v>26.972999999999999</v>
+      </c>
+      <c r="L23">
+        <v>26.917999999999999</v>
+      </c>
+      <c r="M23">
+        <v>26.841999999999999</v>
+      </c>
+      <c r="N23">
+        <v>26.641999999999999</v>
+      </c>
+      <c r="O23">
+        <v>26.471</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>-0.44</v>
+      </c>
+      <c r="C24">
+        <v>-0.439</v>
+      </c>
+      <c r="D24">
+        <v>-0.435</v>
+      </c>
+      <c r="E24">
+        <v>-0.43099999999999999</v>
+      </c>
+      <c r="F24">
+        <v>-0.42599999999999999</v>
+      </c>
+      <c r="G24">
+        <v>-0.42099999999999999</v>
+      </c>
+      <c r="H24">
+        <v>-0.41599999999999998</v>
+      </c>
+      <c r="I24">
+        <v>-0.41399999999999998</v>
+      </c>
+      <c r="J24">
+        <v>-0.40400000000000003</v>
+      </c>
+      <c r="K24">
+        <v>-0.39900000000000002</v>
+      </c>
+      <c r="L24">
+        <v>-0.39100000000000001</v>
+      </c>
+      <c r="M24">
+        <v>-0.38400000000000001</v>
+      </c>
+      <c r="N24">
+        <v>-0.36</v>
+      </c>
+      <c r="O24">
+        <v>-0.33900000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>10</v>
       </c>
-      <c r="B23">
+      <c r="B25">
         <v>0.26800000000000002</v>
       </c>
-      <c r="C23">
+      <c r="C25">
         <v>0.26300000000000001</v>
       </c>
-      <c r="D23">
+      <c r="D25">
         <v>0.26300000000000001</v>
       </c>
-      <c r="E23">
+      <c r="E25">
         <v>0.26300000000000001</v>
       </c>
-      <c r="F23">
+      <c r="F25">
         <v>0.26600000000000001</v>
       </c>
-      <c r="G23">
+      <c r="G25">
         <v>0.26900000000000002</v>
       </c>
-      <c r="H23">
+      <c r="H25">
         <v>0.27200000000000002</v>
       </c>
-      <c r="I23">
+      <c r="I25">
         <v>0.27500000000000002</v>
       </c>
-      <c r="J23">
+      <c r="J25">
         <v>0.28699999999999998</v>
       </c>
-      <c r="K23">
+      <c r="K25">
         <v>0.29599999999999999</v>
       </c>
-      <c r="L23">
+      <c r="L25">
         <v>0.30399999999999999</v>
       </c>
-      <c r="M23">
+      <c r="M25">
         <v>0.318</v>
       </c>
-      <c r="N23">
+      <c r="N25">
         <v>0.47</v>
       </c>
-      <c r="O23">
+      <c r="O25">
         <v>0.376</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>19</v>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auswertung vom ersten tag fertig. temperatur plots fehlen noch
</commit_message>
<xml_diff>
--- a/Versuch424-Hall-Effekt-in-Halbleitern/Report/Tables/Day1-2.xlsx
+++ b/Versuch424-Hall-Effekt-in-Halbleitern/Report/Tables/Day1-2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
   </bookViews>
   <sheets>
     <sheet name="Tag 1 probe 1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="78">
   <si>
     <t>mess nr.</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>T^-1</t>
+  </si>
+  <si>
+    <t>mV</t>
   </si>
 </sst>
 </file>
@@ -1395,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC50"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" topLeftCell="F10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z41" sqref="Z41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2185,6 +2188,9 @@
       <c r="P19" t="s">
         <v>62</v>
       </c>
+      <c r="W19" t="s">
+        <v>77</v>
+      </c>
       <c r="X19" s="7" t="s">
         <v>55</v>
       </c>
@@ -3337,8 +3343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W41" sqref="W41:Y45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5260,7 +5266,7 @@
   <dimension ref="A1:S73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>